<commit_message>
fixed condorcteCriterium and plurality method vote sum
</commit_message>
<xml_diff>
--- a/Votes.xlsx
+++ b/Votes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -262,11 +262,11 @@
   </sheetPr>
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K5" activeCellId="0" sqref="K5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -552,29 +552,29 @@
   </sheetPr>
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>